<commit_message>
Dodan scenarij 5 (lapsus)
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/OdabirPredmeta.xlsx
+++ b/UseCaseIScenarij/OdabirPredmeta.xlsx
@@ -47,9 +47,6 @@
     <t>Proširenja/Alternativa</t>
   </si>
   <si>
-    <t>Scenarij 4:</t>
-  </si>
-  <si>
     <t>\</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>4. Obavještavanje instruktora da ponovo može da pošalje zahtjev za odabir predmeta</t>
+  </si>
+  <si>
+    <t>Scenarij 5:</t>
   </si>
 </sst>
 </file>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,10 +541,10 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -628,80 +628,80 @@
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="8"/>
     </row>
@@ -709,13 +709,13 @@
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="8"/>
     </row>

</xml_diff>